<commit_message>
Create docs No empty project folder
</commit_message>
<xml_diff>
--- a/inst/extdata/examples/TestProject/ProjectConfiguration.xlsx
+++ b/inst/extdata/examples/TestProject/ProjectConfiguration.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felix\Code\esqlabsR\inst\extdata\examples\TestProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\esqlabsR\inst\extdata\examples\TestProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7726BD95-797B-4D1C-9EC3-8915F5BC2AA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9741C233-F0FD-4B06-AE79-DD26FE59A786}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1125" yWindow="2730" windowWidth="17610" windowHeight="13590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-15" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Property</t>
   </si>
@@ -45,12 +45,6 @@
     <t>ModelParameters.xlsx</t>
   </si>
   <si>
-    <t>Path to the folder with pkml simulation files; relative to the "Code" folder</t>
-  </si>
-  <si>
-    <t>Path to the folder with excel files with parametrization; relative to the "Code" folder.</t>
-  </si>
-  <si>
     <t>Name of the excel file with global model parametrization. Must be located in the "paramsFolder"</t>
   </si>
   <si>
@@ -84,9 +78,6 @@
     <t>dataFolder</t>
   </si>
   <si>
-    <t>Path to the folder where experimental data files are located; relative to the "Code" folder</t>
-  </si>
-  <si>
     <t>dataFile</t>
   </si>
   <si>
@@ -102,18 +93,12 @@
     <t>outputFolder</t>
   </si>
   <si>
-    <t>Path to the folder where the results should be saved to; relative to the "Code" folder</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
     <t>compoundPropertiesFile</t>
   </si>
   <si>
-    <t>Compound Properties.xlsx</t>
-  </si>
-  <si>
     <t>Name of data importer configuration file in xml format used to load the data. Must be located in the "dataFolder"</t>
   </si>
   <si>
@@ -151,6 +136,18 @@
   </si>
   <si>
     <t>Results</t>
+  </si>
+  <si>
+    <t>Path to the folder with pkml simulation files; relative to the location of this file</t>
+  </si>
+  <si>
+    <t>Path to the folder with excel files with parametrization; relative to the location of this file</t>
+  </si>
+  <si>
+    <t>Path to the folder where the results should be saved to; relative to the location of this file</t>
+  </si>
+  <si>
+    <t>Path to the folder where experimental data files are located; relative to the location of this file</t>
   </si>
 </sst>
 </file>
@@ -480,7 +477,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -498,7 +495,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -506,10 +503,10 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -517,10 +514,10 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -531,117 +528,114 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
         <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
         <v>14</v>
-      </c>
-      <c r="C7" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" t="s">
         <v>15</v>
-      </c>
-      <c r="B8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C8" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" t="s">
         <v>40</v>
-      </c>
-      <c r="C10" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C14" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rename extension + fix some excel files + add html format rules + add scss style rules
</commit_message>
<xml_diff>
--- a/inst/extdata/examples/TestProject/ProjectConfiguration.xlsx
+++ b/inst/extdata/examples/TestProject/ProjectConfiguration.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\esqlabsR\inst\extdata\examples\TestProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felix\Code\esqlabsR\inst\extdata\examples\TestProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9741C233-F0FD-4B06-AE79-DD26FE59A786}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0006F2FC-DAFD-4808-860D-FB5AE2E93838}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-15" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8790" yWindow="5220" windowWidth="38700" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -108,9 +108,6 @@
     <t>ApplicationParameters.xlsx</t>
   </si>
   <si>
-    <t>TestProject_TimeValuesData.xlsx</t>
-  </si>
-  <si>
     <t>plotsFile</t>
   </si>
   <si>
@@ -148,6 +145,9 @@
   </si>
   <si>
     <t>Path to the folder where experimental data files are located; relative to the location of this file</t>
+  </si>
+  <si>
+    <t>example_TimeValuesData.xlsx</t>
   </si>
 </sst>
 </file>
@@ -477,7 +477,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -503,10 +503,10 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -514,10 +514,10 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -533,10 +533,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" t="s">
         <v>31</v>
-      </c>
-      <c r="B5" t="s">
-        <v>32</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
@@ -577,13 +577,13 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" t="s">
         <v>28</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>29</v>
-      </c>
-      <c r="C9" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -591,10 +591,10 @@
         <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -602,7 +602,7 @@
         <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="C11" t="s">
         <v>18</v>
@@ -632,10 +632,10 @@
         <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -645,6 +645,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010011DB5BA7A27696418C6D2C8B46A68E83" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b6d50ae52c45ae5cf3a9b42a45f9049e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="398d2b5b-77f8-4c5f-a794-3d35ce849315" xmlns:ns3="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f65cf74c317ca0ec831fcb171d38ef6f" ns2:_="" ns3:_="">
     <xsd:import namespace="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
@@ -861,12 +867,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -877,6 +877,15 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE7732FB-5A16-4D8D-B2A0-DAE82353628B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8CE9E921-488E-4950-83CF-BA07CBEDBDF1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -895,15 +904,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE7732FB-5A16-4D8D-B2A0-DAE82353628B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B48AA3D9-A829-4D13-95B1-181AC8A856B4}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
- Fixes #554 (#628)
- Default excel file for population definitions has been renamed from `PopulationParameters.xlsx`
to `Populations.xlsx` (#554, @PavelBal)
- Field `populationParamsFile` of the `ProjectConfiguration` class has been renamed to `populationsFile` (#554, @PavelBal)
</commit_message>
<xml_diff>
--- a/inst/extdata/examples/TestProject/ProjectConfiguration.xlsx
+++ b/inst/extdata/examples/TestProject/ProjectConfiguration.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\esqlabsR\inst\extdata\examples\TestProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9741C233-F0FD-4B06-AE79-DD26FE59A786}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5036F7C4-8EA2-43BE-8F5B-39EB4A57F6E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-15" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -51,12 +51,6 @@
     <t>Name of the excel file with individual-specific model parametrization. Must be located in the "paramsFolder"</t>
   </si>
   <si>
-    <t>populationParamsFile</t>
-  </si>
-  <si>
-    <t>PopulationParameters.xlsx</t>
-  </si>
-  <si>
     <t>Name of the excel file with population information. Must be located in the "paramsFolder"</t>
   </si>
   <si>
@@ -148,6 +142,12 @@
   </si>
   <si>
     <t>Path to the folder where experimental data files are located; relative to the location of this file</t>
+  </si>
+  <si>
+    <t>populationsFile</t>
+  </si>
+  <si>
+    <t>Populations.xlsx</t>
   </si>
 </sst>
 </file>
@@ -477,17 +477,17 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="30.5703125" customWidth="1"/>
+    <col min="1" max="1" width="30.578125" customWidth="1"/>
     <col min="2" max="2" width="38" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="120.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="120.578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -495,32 +495,32 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -531,111 +531,111 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" t="s">
         <v>8</v>
       </c>
-      <c r="B6" t="s">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="C6" t="s">
+      <c r="B7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
         <v>11</v>
       </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="B10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s">
         <v>16</v>
       </c>
-      <c r="B10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" t="s">
         <v>17</v>
       </c>
-      <c r="B11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="B12" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" t="s">
         <v>19</v>
       </c>
-      <c r="B12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>21</v>
-      </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -645,6 +645,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010011DB5BA7A27696418C6D2C8B46A68E83" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b6d50ae52c45ae5cf3a9b42a45f9049e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="398d2b5b-77f8-4c5f-a794-3d35ce849315" xmlns:ns3="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f65cf74c317ca0ec831fcb171d38ef6f" ns2:_="" ns3:_="">
     <xsd:import namespace="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
@@ -861,12 +867,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -877,6 +877,15 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE7732FB-5A16-4D8D-B2A0-DAE82353628B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8CE9E921-488E-4950-83CF-BA07CBEDBDF1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -895,15 +904,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE7732FB-5A16-4D8D-B2A0-DAE82353628B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B48AA3D9-A829-4D13-95B1-181AC8A856B4}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Harmonize Excel configuration files (#633)
</commit_message>
<xml_diff>
--- a/inst/extdata/examples/TestProject/ProjectConfiguration.xlsx
+++ b/inst/extdata/examples/TestProject/ProjectConfiguration.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\esqlabsR\inst\extdata\examples\TestProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felix\Code\esqlabsR\inst\extdata\examples\TestProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9741C233-F0FD-4B06-AE79-DD26FE59A786}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BAC9D92-BF63-409B-97DC-F52C4A754153}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-15" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -39,9 +39,6 @@
     <t>paramsFolder</t>
   </si>
   <si>
-    <t>paramsFile</t>
-  </si>
-  <si>
     <t>ModelParameters.xlsx</t>
   </si>
   <si>
@@ -51,24 +48,12 @@
     <t>Name of the excel file with individual-specific model parametrization. Must be located in the "paramsFolder"</t>
   </si>
   <si>
-    <t>populationParamsFile</t>
-  </si>
-  <si>
-    <t>PopulationParameters.xlsx</t>
-  </si>
-  <si>
     <t>Name of the excel file with population information. Must be located in the "paramsFolder"</t>
   </si>
   <si>
-    <t>scenarioDefinitionFile</t>
-  </si>
-  <si>
     <t>Scenarios.xlsx</t>
   </si>
   <si>
-    <t>scenarioApplicationsFile</t>
-  </si>
-  <si>
     <t>Name of the excel file with scenario definitions. Must be located in the "paramsFolder"</t>
   </si>
   <si>
@@ -105,9 +90,6 @@
     <t>Path to the excel file containing information about all compounds in the model. Must be located in the "dataFolder"</t>
   </si>
   <si>
-    <t>ApplicationParameters.xlsx</t>
-  </si>
-  <si>
     <t>TestProject_TimeValuesData.xlsx</t>
   </si>
   <si>
@@ -126,18 +108,6 @@
     <t>Individuals.xlsx</t>
   </si>
   <si>
-    <t>Models/Simulations</t>
-  </si>
-  <si>
-    <t>Parameters</t>
-  </si>
-  <si>
-    <t>Data</t>
-  </si>
-  <si>
-    <t>Results</t>
-  </si>
-  <si>
     <t>Path to the folder with pkml simulation files; relative to the location of this file</t>
   </si>
   <si>
@@ -148,6 +118,36 @@
   </si>
   <si>
     <t>Path to the folder where experimental data files are located; relative to the location of this file</t>
+  </si>
+  <si>
+    <t>modelParamsFile</t>
+  </si>
+  <si>
+    <t>scenariosFile</t>
+  </si>
+  <si>
+    <t>Populations.xlsx</t>
+  </si>
+  <si>
+    <t>populationsFile</t>
+  </si>
+  <si>
+    <t>applicationsFile</t>
+  </si>
+  <si>
+    <t>Parameters/</t>
+  </si>
+  <si>
+    <t>Models/Simulations/</t>
+  </si>
+  <si>
+    <t>Data/</t>
+  </si>
+  <si>
+    <t>Results/</t>
+  </si>
+  <si>
+    <t>Applications.xlsx</t>
   </si>
 </sst>
 </file>
@@ -477,7 +477,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -495,7 +495,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -503,10 +503,10 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -514,128 +514,128 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C10" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
         <v>19</v>
-      </c>
-      <c r="B12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C13" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C14" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -645,6 +645,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010011DB5BA7A27696418C6D2C8B46A68E83" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b6d50ae52c45ae5cf3a9b42a45f9049e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="398d2b5b-77f8-4c5f-a794-3d35ce849315" xmlns:ns3="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f65cf74c317ca0ec831fcb171d38ef6f" ns2:_="" ns3:_="">
     <xsd:import namespace="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
@@ -861,12 +867,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -877,6 +877,15 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE7732FB-5A16-4D8D-B2A0-DAE82353628B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8CE9E921-488E-4950-83CF-BA07CBEDBDF1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -895,15 +904,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE7732FB-5A16-4D8D-B2A0-DAE82353628B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B48AA3D9-A829-4D13-95B1-181AC8A856B4}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
renamed the `Parameters` folder to `Configurations` (#631)
</commit_message>
<xml_diff>
--- a/inst/extdata/examples/TestProject/ProjectConfiguration.xlsx
+++ b/inst/extdata/examples/TestProject/ProjectConfiguration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felix\Code\esqlabsR\inst\extdata\examples\TestProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BAC9D92-BF63-409B-97DC-F52C4A754153}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A8203D5-46EA-4C7B-A046-B7983FA233A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,9 +36,6 @@
     <t>modelFolder</t>
   </si>
   <si>
-    <t>paramsFolder</t>
-  </si>
-  <si>
     <t>ModelParameters.xlsx</t>
   </si>
   <si>
@@ -135,9 +132,6 @@
     <t>applicationsFile</t>
   </si>
   <si>
-    <t>Parameters/</t>
-  </si>
-  <si>
     <t>Models/Simulations/</t>
   </si>
   <si>
@@ -148,6 +142,12 @@
   </si>
   <si>
     <t>Applications.xlsx</t>
+  </si>
+  <si>
+    <t>Configurations/</t>
+  </si>
+  <si>
+    <t>configurationsFolder</t>
   </si>
 </sst>
 </file>
@@ -477,7 +477,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -495,7 +495,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -503,139 +503,139 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>40</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
         <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
         <v>25</v>
       </c>
-      <c r="B5" t="s">
-        <v>26</v>
-      </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
         <v>8</v>
-      </c>
-      <c r="C7" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
         <v>22</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>23</v>
-      </c>
-      <c r="C9" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
         <v>12</v>
-      </c>
-      <c r="B11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
         <v>14</v>
       </c>
-      <c r="B12" t="s">
-        <v>15</v>
-      </c>
       <c r="C12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add populationsCSV path in projectConfiguration + use projectConfiguration$populationsCSV to locate population CSV files to read + add test to make sure all test scenarios can be properly created
</commit_message>
<xml_diff>
--- a/inst/extdata/examples/TestProject/ProjectConfiguration.xlsx
+++ b/inst/extdata/examples/TestProject/ProjectConfiguration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felix\Code\esqlabsR\inst\extdata\examples\TestProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A8203D5-46EA-4C7B-A046-B7983FA233A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A794A8C-6F41-46F9-8B87-F8984D1AF5C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>Property</t>
   </si>
@@ -148,6 +148,15 @@
   </si>
   <si>
     <t>configurationsFolder</t>
+  </si>
+  <si>
+    <t>populationsCSV</t>
+  </si>
+  <si>
+    <t>PopulationsCSV</t>
+  </si>
+  <si>
+    <t>Name of the folder containing population defined in files</t>
   </si>
 </sst>
 </file>
@@ -474,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -555,86 +564,97 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>15</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>37</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C15" t="s">
         <v>28</v>
       </c>
     </row>
@@ -645,12 +665,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010011DB5BA7A27696418C6D2C8B46A68E83" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b6d50ae52c45ae5cf3a9b42a45f9049e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="398d2b5b-77f8-4c5f-a794-3d35ce849315" xmlns:ns3="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f65cf74c317ca0ec831fcb171d38ef6f" ns2:_="" ns3:_="">
     <xsd:import namespace="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
@@ -867,6 +881,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -877,15 +897,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE7732FB-5A16-4D8D-B2A0-DAE82353628B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8CE9E921-488E-4950-83CF-BA07CBEDBDF1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -904,6 +915,15 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE7732FB-5A16-4D8D-B2A0-DAE82353628B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B48AA3D9-A829-4D13-95B1-181AC8A856B4}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Remove compound property in ProjectConfiguration excel file + replace leftover previous name
</commit_message>
<xml_diff>
--- a/inst/extdata/examples/TestProject/ProjectConfiguration.xlsx
+++ b/inst/extdata/examples/TestProject/ProjectConfiguration.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felix\Code\esqlabsR\inst\extdata\examples\TestProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A794A8C-6F41-46F9-8B87-F8984D1AF5C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E72E23CF-E5C4-4D14-ACE1-B1E19FC9A486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>Property</t>
   </si>
@@ -78,15 +78,9 @@
     <t>Description</t>
   </si>
   <si>
-    <t>compoundPropertiesFile</t>
-  </si>
-  <si>
     <t>Name of data importer configuration file in xml format used to load the data. Must be located in the "dataFolder"</t>
   </si>
   <si>
-    <t>Path to the excel file containing information about all compounds in the model. Must be located in the "dataFolder"</t>
-  </si>
-  <si>
     <t>TestProject_TimeValuesData.xlsx</t>
   </si>
   <si>
@@ -150,13 +144,13 @@
     <t>configurationsFolder</t>
   </si>
   <si>
-    <t>populationsCSV</t>
-  </si>
-  <si>
     <t>PopulationsCSV</t>
   </si>
   <si>
     <t>Name of the folder containing population defined in files</t>
+  </si>
+  <si>
+    <t>populationsFolder</t>
   </si>
 </sst>
 </file>
@@ -483,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -512,26 +506,26 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
@@ -542,10 +536,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -553,10 +547,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
@@ -567,15 +561,15 @@
         <v>41</v>
       </c>
       <c r="B7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
@@ -586,10 +580,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C9" t="s">
         <v>9</v>
@@ -597,13 +591,13 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
         <v>21</v>
-      </c>
-      <c r="B10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -611,10 +605,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -622,7 +616,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C12" t="s">
         <v>12</v>
@@ -636,26 +630,18 @@
         <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>15</v>
+      </c>
+      <c r="B14" t="s">
+        <v>35</v>
       </c>
       <c r="C14" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Restore populationsFolder to populationCSV
</commit_message>
<xml_diff>
--- a/inst/extdata/examples/TestProject/ProjectConfiguration.xlsx
+++ b/inst/extdata/examples/TestProject/ProjectConfiguration.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felix\Code\esqlabsR\inst\extdata\examples\TestProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E72E23CF-E5C4-4D14-ACE1-B1E19FC9A486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32177ECF-6B11-41E0-91F7-7EBCAFE9CDEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -150,7 +150,7 @@
     <t>Name of the folder containing population defined in files</t>
   </si>
   <si>
-    <t>populationsFolder</t>
+    <t>populationsCSV</t>
   </si>
 </sst>
 </file>
@@ -480,7 +480,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -651,6 +651,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010011DB5BA7A27696418C6D2C8B46A68E83" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b6d50ae52c45ae5cf3a9b42a45f9049e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="398d2b5b-77f8-4c5f-a794-3d35ce849315" xmlns:ns3="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f65cf74c317ca0ec831fcb171d38ef6f" ns2:_="" ns3:_="">
     <xsd:import namespace="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
@@ -867,22 +882,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B48AA3D9-A829-4D13-95B1-181AC8A856B4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE7732FB-5A16-4D8D-B2A0-DAE82353628B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8CE9E921-488E-4950-83CF-BA07CBEDBDF1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -899,21 +916,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE7732FB-5A16-4D8D-B2A0-DAE82353628B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B48AA3D9-A829-4D13-95B1-181AC8A856B4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Rename Population Folder ProjectConfiguration property - Property is named populationsFolder - Project template folder contains populations is named PopulationsCSV
</commit_message>
<xml_diff>
--- a/inst/extdata/examples/TestProject/ProjectConfiguration.xlsx
+++ b/inst/extdata/examples/TestProject/ProjectConfiguration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felix\Code\esqlabsR\inst\extdata\examples\TestProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32177ECF-6B11-41E0-91F7-7EBCAFE9CDEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D3F1CFE-4194-4F40-89A3-32F8309FE566}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -150,7 +150,7 @@
     <t>Name of the folder containing population defined in files</t>
   </si>
   <si>
-    <t>populationsCSV</t>
+    <t>populationsFolder</t>
   </si>
 </sst>
 </file>
@@ -651,21 +651,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010011DB5BA7A27696418C6D2C8B46A68E83" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b6d50ae52c45ae5cf3a9b42a45f9049e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="398d2b5b-77f8-4c5f-a794-3d35ce849315" xmlns:ns3="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f65cf74c317ca0ec831fcb171d38ef6f" ns2:_="" ns3:_="">
     <xsd:import namespace="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
@@ -882,24 +867,22 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B48AA3D9-A829-4D13-95B1-181AC8A856B4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE7732FB-5A16-4D8D-B2A0-DAE82353628B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8CE9E921-488E-4950-83CF-BA07CBEDBDF1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -916,4 +899,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE7732FB-5A16-4D8D-B2A0-DAE82353628B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B48AA3D9-A829-4D13-95B1-181AC8A856B4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>